<commit_message>
Add DefaultAttr & AliasAttr
</commit_message>
<xml_diff>
--- a/Demo/Data/0_no_loc/data/Alias.xlsx
+++ b/Demo/Data/0_no_loc/data/Alias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fancyHub\ExportExcel\Demo\Data\0_no_loc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E436D4E3-E25C-4F6A-B32C-C1B526D7583A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD96FA6-0BA9-45EF-A970-895CCE2E4979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="@Alias_XX" sheetId="1" r:id="rId1"/>
@@ -25,66 +25,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
-  <si>
-    <t>SheetName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ColumnName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CodeType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Client</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Server</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Csharp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ItemData</t>
+    <t>PairItemIntInt64</t>
+  </si>
+  <si>
+    <t>UnityEngine.Vector3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Go</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*gmath.Vector3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x|y|z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fields</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cpp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id|Exist</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>PairItemIntBool</t>
-  </si>
-  <si>
-    <t>PairItemIntBool</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PairField2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PairField3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PairItemIntInt64</t>
-  </si>
-  <si>
-    <t>PairFieldList2</t>
-  </si>
-  <si>
-    <t>TestComposeKey</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>UnityEngine.Vector3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Id|Value</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -410,93 +400,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.25" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
     <col min="2" max="2" width="18.625" customWidth="1"/>
     <col min="3" max="3" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="25.75" customWidth="1"/>
+    <col min="4" max="4" width="25.75" customWidth="1"/>
+    <col min="5" max="5" width="18.875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>